<commit_message>
update cash and bank account"
</commit_message>
<xml_diff>
--- a/database/seeders/data/Currency.xlsx
+++ b/database/seeders/data/Currency.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>THB</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>is_active</t>
   </si>
 </sst>
 </file>
@@ -400,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -412,7 +415,7 @@
     <col min="3" max="3" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -422,8 +425,11 @@
       <c r="C1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2">
         <v>1</v>
       </c>
@@ -433,8 +439,11 @@
       <c r="C2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1">
       <c r="A3">
         <v>2</v>
       </c>
@@ -444,8 +453,11 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1">
       <c r="A4">
         <v>3</v>
       </c>
@@ -455,8 +467,11 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1">
       <c r="A5">
         <v>4</v>
       </c>
@@ -466,8 +481,11 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1">
       <c r="A6">
         <v>5</v>
       </c>
@@ -477,8 +495,11 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1">
       <c r="A7">
         <v>6</v>
       </c>
@@ -488,8 +509,11 @@
       <c r="C7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1">
       <c r="A8">
         <v>7</v>
       </c>
@@ -499,8 +523,11 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1">
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1">
       <c r="A9">
         <v>8</v>
       </c>
@@ -510,10 +537,13 @@
       <c r="C9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1"/>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>